<commit_message>
About to start trial 2
</commit_message>
<xml_diff>
--- a/Models.xlsx
+++ b/Models.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FA67EB-1239-F844-AEBF-B9267D68BBF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Model</t>
   </si>
@@ -45,13 +46,22 @@
     <t>Adam</t>
   </si>
   <si>
-    <t>66.58% - Epoch 10</t>
+    <t>Simple_MLP([40*(2*context_size+1), 256, 128, 71]) + Softmax</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>66.68% - Epoch 11</t>
+  </si>
+  <si>
+    <t>65% Epoch 5, 66.48% Epoch 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -86,7 +96,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -363,22 +373,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="46.109375" customWidth="1"/>
+    <col min="2" max="2" width="50.33203125" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="30.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -397,8 +409,11 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -415,7 +430,27 @@
         <v>1E-4</v>
       </c>
       <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trying to change batch size
</commit_message>
<xml_diff>
--- a/Models.xlsx
+++ b/Models.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA5D32D-5802-E544-890C-96BDF29357AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2FF9B8-BF5E-E44B-B838-FBEA214BD9CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6080" yWindow="2740" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Model</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t>20.84% - Epoch2</t>
+  </si>
+  <si>
+    <t>29.24% - Epoch 5</t>
+  </si>
+  <si>
+    <t>Can't seem to train with softmax</t>
   </si>
 </sst>
 </file>
@@ -388,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -522,6 +528,23 @@
       <c r="E5" s="1">
         <v>2.0000000000000001E-4</v>
       </c>
+      <c r="F5" s="3">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update readme. Output generation
</commit_message>
<xml_diff>
--- a/Models.xlsx
+++ b/Models.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998E486D-1DE5-D445-81A0-2488C3F72548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="504" windowWidth="28800" windowHeight="17496"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>Model</t>
   </si>
@@ -85,12 +86,18 @@
   </si>
   <si>
     <t>Initial Learning Rate</t>
+  </si>
+  <si>
+    <t>66.80% - Epoch 30</t>
+  </si>
+  <si>
+    <t>Restarted at 16th epoch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -127,7 +134,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -404,25 +411,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="2" max="2" width="50.33203125" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
-    <col min="6" max="7" width="14.109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="6" max="7" width="14.1640625" style="3" customWidth="1"/>
     <col min="8" max="8" width="16.6640625" customWidth="1"/>
-    <col min="9" max="9" width="30.44140625" customWidth="1"/>
+    <col min="9" max="9" width="30.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -451,7 +458,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -480,7 +487,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -509,7 +516,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -535,7 +542,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -564,7 +571,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -584,7 +591,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -610,7 +617,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -627,6 +634,35 @@
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="F8" s="3">
+        <v>256</v>
+      </c>
+      <c r="G8" s="3">
+        <v>30</v>
+      </c>
+      <c r="H8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="F9" s="3">
         <v>256</v>
       </c>
     </row>

</xml_diff>

<commit_message>
prepared for trial 7
</commit_message>
<xml_diff>
--- a/Models.xlsx
+++ b/Models.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998E486D-1DE5-D445-81A0-2488C3F72548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0BEDF5-5859-ED40-BA32-9639AA432A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>Model</t>
   </si>
@@ -92,6 +92,15 @@
   </si>
   <si>
     <t>Restarted at 16th epoch</t>
+  </si>
+  <si>
+    <t>~66%</t>
+  </si>
+  <si>
+    <t>Reached best pretty soon and started to bounce around</t>
+  </si>
+  <si>
+    <t>Simple_MLP([40*(2*context_size+1), 256, 128, 128, 71])</t>
   </si>
 </sst>
 </file>
@@ -412,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -648,7 +657,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>7</v>
+        <v>6.5</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
@@ -663,6 +672,35 @@
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="F9" s="3">
+        <v>256</v>
+      </c>
+      <c r="G9" s="3">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="F10" s="3">
         <v>256</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixing a softmax issue of unknown origin
</commit_message>
<xml_diff>
--- a/Models.xlsx
+++ b/Models.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0BEDF5-5859-ED40-BA32-9639AA432A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F87B52-52F5-EB41-ADC3-694C2168E82F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4940" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
   <si>
     <t>Model</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>Simple_MLP([40*(2*context_size+1), 256, 128, 128, 71])</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -421,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -704,6 +707,11 @@
         <v>256</v>
       </c>
     </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>